<commit_message>
Update app, dataset and add pseudocode html
</commit_message>
<xml_diff>
--- a/dataset_id3_MBG_100_final.xlsx
+++ b/dataset_id3_MBG_100_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuli ahh__\TUGASSSS\Semester 7\KECERDASAN BUATAN\Aplikasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{188DB786-64FA-42B8-800F-62172F286C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA9BCB-8572-4EE3-BC58-394DFAAE0E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -550,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,25 +571,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,38 +636,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2994,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441656EC-41FF-4229-9A71-B7421BD6D9BC}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,16 +3027,16 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="G5" s="27" t="s">
+      <c r="D5" s="29"/>
+      <c r="G5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
       <c r="L5" s="3" t="s">
         <v>73</v>
       </c>
@@ -3056,23 +3051,23 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="G6" s="30" t="s">
+      <c r="D6" s="31"/>
+      <c r="G6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-      <c r="L6" s="33" t="s">
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="L6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="20" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3080,34 +3075,34 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="L7" s="33" t="s">
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="L7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="18" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="L8" s="33" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="L8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="18" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3115,13 +3110,13 @@
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N9" s="18" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3129,13 +3124,13 @@
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N10" s="18" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3160,14 +3155,13 @@
       <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12" t="s">
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="15"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -3182,21 +3176,16 @@
       <c r="D14" s="5">
         <v>59</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15" t="s">
+      <c r="H14" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="15"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -3211,19 +3200,13 @@
       <c r="D15" s="5">
         <v>41</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="19" t="s">
+      <c r="H15" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="15"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -3238,80 +3221,59 @@
       <c r="D16" s="4">
         <v>100</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15" t="s">
+      <c r="H16" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15" t="s">
+      <c r="H17" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="13"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="24"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="I20" s="7"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -3331,16 +3293,15 @@
       <c r="H21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12" t="s">
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="10"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -3353,23 +3314,18 @@
       <c r="D22" s="5">
         <v>59</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15" t="s">
+      <c r="H22" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
@@ -3382,21 +3338,15 @@
       <c r="D23" s="5">
         <v>41</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="19" t="s">
+      <c r="H23" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="15"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -3409,79 +3359,58 @@
       <c r="D24" s="4">
         <v>100</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15" t="s">
+      <c r="H24" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="15"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15" t="s">
+      <c r="H25" t="s">
         <v>53</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="15"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="15"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="13"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="15"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="24"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="N28" s="15"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
@@ -3501,16 +3430,15 @@
       <c r="H29" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12" t="s">
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="15"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L29" s="10"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
@@ -3523,23 +3451,18 @@
       <c r="D30" s="5">
         <v>36</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15" t="s">
+      <c r="H30" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="16" t="s">
+      <c r="K30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="15"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="15"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>16</v>
       </c>
@@ -3552,21 +3475,15 @@
       <c r="D31" s="5">
         <v>64</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="19" t="s">
+      <c r="H31" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="15"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
@@ -3579,79 +3496,58 @@
       <c r="D32" s="4">
         <v>100</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15" t="s">
+      <c r="H32" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="15"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15" t="s">
+      <c r="H33" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="15"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="13"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="F35" s="39" t="s">
+      <c r="F35" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="15"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="24"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="N36" s="15"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>3</v>
       </c>
@@ -3671,16 +3567,15 @@
       <c r="H37" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12" t="s">
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="15"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L37" s="10"/>
+      <c r="M37" s="12"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>17</v>
       </c>
@@ -3693,23 +3588,18 @@
       <c r="D38" s="5">
         <v>48</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15" t="s">
+      <c r="H38" t="s">
         <v>26</v>
       </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="16" t="s">
+      <c r="K38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L38" s="15"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="15"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
@@ -3722,21 +3612,15 @@
       <c r="D39" s="5">
         <v>52</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F39" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="15"/>
-      <c r="H39" s="19" t="s">
+      <c r="H39" t="s">
         <v>66</v>
       </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="15"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>22</v>
       </c>
@@ -3749,63 +3633,41 @@
       <c r="D40" s="4">
         <v>100</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15" t="s">
+      <c r="H40" t="s">
         <v>67</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="15"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F41" s="14" t="s">
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F41" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15" t="s">
+      <c r="H41" t="s">
         <v>69</v>
       </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="15"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F42" s="14"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="15"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="39" t="s">
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="13"/>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="15"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N44" s="15"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="24"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -3819,54 +3681,40 @@
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="11"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="15"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="12"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="5">
         <v>9</v>
       </c>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="F46" s="14" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="F46" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="15"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K46" s="7"/>
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="5">
         <v>4</v>
       </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="15"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="F47" s="13"/>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>22</v>
       </c>
@@ -3875,54 +3723,38 @@
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="15"/>
-    </row>
-    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F49" s="14" t="s">
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F49" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="15"/>
-    </row>
-    <row r="50" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="15"/>
-    </row>
-    <row r="51" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F51" s="39" t="s">
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="15"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="17"/>
+    </row>
+    <row r="51" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="15"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>